<commit_message>
added bunch of random things
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/recap/tender.xlsx
+++ b/CustomLabelPrinter/recap/tender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\eclipse-workspace\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\recap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83B9D98-2151-499F-A201-A89CB0E2D1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BFF3A3-5EF0-4ECE-9A81-A6D1EB635D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17310" yWindow="1320" windowWidth="23280" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENDER" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Date:</t>
+  </si>
+  <si>
+    <t>2nd</t>
   </si>
 </sst>
 </file>
@@ -81,13 +84,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -106,6 +102,12 @@
     <font>
       <b/>
       <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -336,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -347,14 +349,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -362,45 +357,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -418,6 +406,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,10 +694,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:P50"/>
+  <dimension ref="B1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="50" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D46"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -717,97 +708,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-    </row>
-    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C2" s="18" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="17"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="2:16" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>17</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>18</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>19</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="8">
         <v>20</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="8">
         <v>21</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>22</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="8">
         <v>23</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="8">
         <v>24</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="8">
         <v>25</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="26"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="30"/>
-      <c r="C5" s="21">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19">
         <v>15686</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -817,31 +808,31 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="36"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="30"/>
     </row>
     <row r="6" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="32"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -851,16 +842,16 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="34"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30"/>
-      <c r="C8" s="21">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19">
         <v>10146</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -870,82 +861,82 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="36"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="30"/>
     </row>
     <row r="9" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="30"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="32"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="30"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="32"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="26"/>
     </row>
     <row r="11" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="30"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="32"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="12" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="30"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="32"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -955,16 +946,16 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="34"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
-      <c r="C14" s="21">
+      <c r="B14" s="18"/>
+      <c r="C14" s="19">
         <v>21108</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -974,84 +965,84 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="36"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="30"/>
     </row>
     <row r="15" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="32"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="30"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="32"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="32"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="30"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="32"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="30"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1061,16 +1052,16 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="34"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="28"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
-      <c r="C20" s="21">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19">
         <v>15799</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1080,31 +1071,31 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="36"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="30"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="30"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="32"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1114,16 +1105,16 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="34"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="30"/>
-      <c r="C23" s="21">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19">
         <v>15734</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1133,31 +1124,31 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="36"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="30"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="30"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="32"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="4"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1167,14 +1158,14 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="34"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="30"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1184,31 +1175,31 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="36"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="30"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="32"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="26"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1218,14 +1209,14 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="34"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="28"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="30"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1235,31 +1226,31 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="36"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="30"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="30"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="32"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="26"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1269,16 +1260,16 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="34"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="28"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="30"/>
-      <c r="C32" s="21">
+      <c r="B32" s="18"/>
+      <c r="C32" s="19">
         <v>10178</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="6"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1288,31 +1279,31 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="36"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="30"/>
     </row>
     <row r="33" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="30"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="32"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="26"/>
     </row>
     <row r="34" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -1322,16 +1313,16 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="34"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="28"/>
     </row>
     <row r="35" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="30"/>
-      <c r="C35" s="21">
+      <c r="B35" s="18"/>
+      <c r="C35" s="19">
         <v>23408</v>
       </c>
-      <c r="D35" s="22"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="6"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1341,31 +1332,31 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="36"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="30"/>
     </row>
     <row r="36" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="30"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="32"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="26"/>
     </row>
     <row r="37" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -1375,16 +1366,16 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="34"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="28"/>
     </row>
     <row r="38" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="30"/>
-      <c r="C38" s="21">
+      <c r="B38" s="18"/>
+      <c r="C38" s="19">
         <v>21872</v>
       </c>
-      <c r="D38" s="22"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -1394,31 +1385,31 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="36"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="30"/>
     </row>
     <row r="39" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="30"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="31"/>
-      <c r="P39" s="32"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="26"/>
     </row>
     <row r="40" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="30"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -1428,16 +1419,16 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="16"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="34"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="28"/>
     </row>
     <row r="41" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="30"/>
-      <c r="C41" s="21">
+      <c r="B41" s="18"/>
+      <c r="C41" s="19">
         <v>10195</v>
       </c>
-      <c r="D41" s="22"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="6"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -1447,31 +1438,31 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="36"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="30"/>
     </row>
     <row r="42" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="30"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="31"/>
-      <c r="P42" s="32"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="26"/>
     </row>
     <row r="43" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="24"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -1481,14 +1472,14 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="34"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="28"/>
     </row>
     <row r="44" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="30"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="22"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="6"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -1498,30 +1489,30 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="35"/>
-      <c r="P44" s="36"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="30"/>
     </row>
     <row r="45" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="30"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="32"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="26"/>
     </row>
     <row r="46" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -1531,13 +1522,13 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
-      <c r="N46" s="16"/>
-      <c r="O46" s="33"/>
-      <c r="P46" s="34"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="28"/>
     </row>
     <row r="47" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="21"/>
-      <c r="D47" s="22"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="6"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -1547,29 +1538,29 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="5"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="32"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="26"/>
     </row>
     <row r="48" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="23"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="31"/>
-      <c r="P48" s="32"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="26"/>
     </row>
     <row r="49" spans="3:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="19"/>
-      <c r="D49" s="20"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -1579,28 +1570,12 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="34"/>
-    </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="27"/>
+      <c r="P49" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
     <mergeCell ref="O47:P49"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="O29:P31"/>
@@ -1642,6 +1617,7 @@
     <mergeCell ref="C9:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D19"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>

</xml_diff>